<commit_message>
Probably well documented application
</commit_message>
<xml_diff>
--- a/Documentation/KNN_Tests.xlsx
+++ b/Documentation/KNN_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radu\Desktop\Licenta\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D14D6FA-E5C3-490A-A891-5F6B0FD3201C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94BC6E-B5C7-458A-8CAD-5A39CB060885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{BBC9B454-0FF0-45FB-87B7-720F0AD6F11C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="25">
   <si>
     <t>Metrica</t>
   </si>
@@ -76,6 +76,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>100 teste, cosine, pentru fiecare k</t>
+  </si>
+  <si>
+    <t>100 teste, euclidiană, pentru fiecare k</t>
+  </si>
+  <si>
+    <t>100 teste, Jaccard, pentru fiecare k</t>
+  </si>
+  <si>
+    <t>VH%</t>
+  </si>
+  <si>
+    <t>H%</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>100 teste, k=[3, 5,  7, 11, 110]</t>
+  </si>
+  <si>
+    <t>100 teste, pentru fiecare metrică</t>
   </si>
 </sst>
 </file>
@@ -221,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -235,21 +259,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -257,6 +266,27 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -277,479 +307,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cosine</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9280</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9958</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34223</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>145111</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>454228</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>652800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C95F-4340-92E1-819BC1F23B84}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Euclidiană</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$5:$H$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3045</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>86596</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>511789</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49470</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>652800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C95F-4340-92E1-819BC1F23B84}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Jaccard</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3960</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16443</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>148263</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>479434</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>652800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C95F-4340-92E1-819BC1F23B84}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1913128496"/>
-        <c:axId val="1913121776"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1913128496"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1913121776"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1913121776"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1913128496"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1388,556 +945,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k=3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$R$2:$W$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$4:$W$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2745</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13797</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19740</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3930</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B191-44DA-A76F-B40A930BFC01}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k=5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$R$2:$W$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$5:$W$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3035</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3540</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35238</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9287</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>72000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B191-44DA-A76F-B40A930BFC01}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k=7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$R$2:$W$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$6:$W$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3039</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3794</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26209</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>51869</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15889</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B191-44DA-A76F-B40A930BFC01}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k=11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$R$2:$W$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Very High</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>High</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Moderate</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Very Low</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$7:$W$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3039</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3812</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32539</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>88163</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30847</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>158400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B191-44DA-A76F-B40A930BFC01}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1668600096"/>
-        <c:axId val="1668598176"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1668600096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1668598176"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1668598176"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1668600096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3020,6 +2028,993 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1660943984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cosine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9280</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34223</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>454228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-271E-4A8A-A3FD-FDD5F7D46F19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Euclidiană</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3045</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>511789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-271E-4A8A-A3FD-FDD5F7D46F19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jaccard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3960</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>148263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>479434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-271E-4A8A-A3FD-FDD5F7D46F19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1769993503"/>
+        <c:axId val="1769995903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1769993503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769995903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1769995903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769993503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k=3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19740</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3930</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BFAC-467E-92E0-6510C82327CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$5:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3035</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3540</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9287</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BFAC-467E-92E0-6510C82327CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k=7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$6:$V$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26209</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51869</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BFAC-467E-92E0-6510C82327CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k=11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Very High</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>High</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Moderate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Low</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Very Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$7:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32539</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88163</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30847</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BFAC-467E-92E0-6510C82327CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1768330303"/>
+        <c:axId val="1768323103"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1768330303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768323103"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1768323103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768330303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3770,7 +3765,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3974,22 +3969,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4094,8 +4090,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4227,19 +4223,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4776,7 +4773,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4980,23 +4977,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5101,8 +5097,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5234,20 +5230,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5282,42 +5277,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>151447</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>532447</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A984F7-1C85-D2CE-8049-6A55CC106E5F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -5348,43 +5307,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>149543</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>37148</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{446A69DA-98FD-18F4-8842-FB60B38C42B6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5409,6 +5332,78 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86A03191-A751-B582-D869-445AD37BF8CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>184785</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8826CB-0195-1660-65C3-A511BB4E6E14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>534352</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180023</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>63818</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C79C5E0-FB1A-839D-6E0E-327FEE2928D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5726,49 +5721,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE160EFE-F876-4D4E-9FAF-8DB9D1099C07}">
-  <dimension ref="B1:W60"/>
+  <dimension ref="B1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="M10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="9"/>
-      <c r="Q2" s="5" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="12"/>
+      <c r="Q2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="9"/>
     </row>
-    <row r="3" spans="2:23" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6"/>
+    <row r="3" spans="2:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5784,10 +5769,7 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5806,7 +5788,7 @@
       <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="6"/>
+      <c r="Q3" s="9"/>
       <c r="R3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5822,11 +5804,8 @@
       <c r="V3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -5845,9 +5824,6 @@
       <c r="G4" s="4">
         <v>454228</v>
       </c>
-      <c r="H4" s="4">
-        <v>652800</v>
-      </c>
       <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
@@ -5887,11 +5863,8 @@
       <c r="V4" s="4">
         <v>3930</v>
       </c>
-      <c r="W4" s="4">
-        <v>43200</v>
-      </c>
     </row>
-    <row r="5" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -5910,9 +5883,6 @@
       <c r="G5" s="4">
         <v>49470</v>
       </c>
-      <c r="H5" s="4">
-        <v>652800</v>
-      </c>
       <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
@@ -5952,11 +5922,8 @@
       <c r="V5" s="4">
         <v>9287</v>
       </c>
-      <c r="W5" s="4">
-        <v>72000</v>
-      </c>
     </row>
-    <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5975,9 +5942,6 @@
       <c r="G6" s="4">
         <v>479434</v>
       </c>
-      <c r="H6" s="4">
-        <v>652800</v>
-      </c>
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
@@ -6017,11 +5981,8 @@
       <c r="V6" s="4">
         <v>15889</v>
       </c>
-      <c r="W6" s="4">
-        <v>100800</v>
-      </c>
     </row>
-    <row r="7" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
@@ -6061,11 +6022,8 @@
       <c r="V7" s="4">
         <v>30847</v>
       </c>
-      <c r="W7" s="4">
-        <v>158400</v>
-      </c>
     </row>
-    <row r="8" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
@@ -6090,33 +6048,33 @@
     </row>
     <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="J32" s="5" t="s">
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="J32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K32" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="9"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="12"/>
     </row>
     <row r="33" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="1" t="s">
         <v>1</v>
       </c>
@@ -6132,8 +6090,8 @@
       <c r="H33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
       <c r="L33" s="1" t="s">
         <v>1</v>
       </c>
@@ -6339,18 +6297,18 @@
       <c r="H38" s="4">
         <v>0</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L38" s="8"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="9"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="12"/>
     </row>
     <row r="39" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
@@ -6374,8 +6332,8 @@
       <c r="H39" s="4">
         <v>4804</v>
       </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
       <c r="L39" s="1" t="s">
         <v>1</v>
       </c>
@@ -6395,7 +6353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
@@ -6581,18 +6539,18 @@
       <c r="H44" s="4">
         <v>0</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L44" s="8"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="9"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="12"/>
     </row>
     <row r="45" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
@@ -6616,8 +6574,8 @@
       <c r="H45" s="4">
         <v>16238</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
       <c r="L45" s="1" t="s">
         <v>1</v>
       </c>
@@ -6638,25 +6596,25 @@
       </c>
     </row>
     <row r="46" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="6">
         <v>1867</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="7">
         <v>2252</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46" s="7">
         <v>9086</v>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="7">
         <v>89176</v>
       </c>
-      <c r="H46" s="12">
+      <c r="H46" s="7">
         <v>425619</v>
       </c>
       <c r="J46" s="2">
@@ -6685,7 +6643,7 @@
       </c>
     </row>
     <row r="47" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -6732,7 +6690,7 @@
       </c>
     </row>
     <row r="48" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -6780,22 +6738,22 @@
     </row>
     <row r="49" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J50" s="5" t="s">
+      <c r="J50" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K50" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L50" s="8"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="9"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="12"/>
     </row>
     <row r="51" spans="10:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
       <c r="L51" s="1" t="s">
         <v>1</v>
       </c>
@@ -6815,7 +6773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="10:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J52" s="2">
         <v>11</v>
       </c>
@@ -6841,7 +6799,7 @@
         <v>52800</v>
       </c>
     </row>
-    <row r="53" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="10:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J53" s="2">
         <v>11</v>
       </c>
@@ -6895,22 +6853,22 @@
     </row>
     <row r="55" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J56" s="5" t="s">
+      <c r="J56" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K56" s="5" t="s">
+      <c r="K56" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L56" s="8"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="9"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="12"/>
     </row>
     <row r="57" spans="10:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
       <c r="L57" s="1" t="s">
         <v>1</v>
       </c>
@@ -6931,28 +6889,28 @@
       </c>
     </row>
     <row r="58" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J58" s="10">
+      <c r="J58" s="5">
         <v>110</v>
       </c>
-      <c r="K58" s="11" t="s">
+      <c r="K58" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L58" s="11">
+      <c r="L58" s="6">
         <v>1867</v>
       </c>
-      <c r="M58" s="12">
+      <c r="M58" s="7">
         <v>2252</v>
       </c>
-      <c r="N58" s="12">
+      <c r="N58" s="7">
         <v>9086</v>
       </c>
-      <c r="O58" s="12">
+      <c r="O58" s="7">
         <v>89176</v>
       </c>
-      <c r="P58" s="12">
+      <c r="P58" s="7">
         <v>425619</v>
       </c>
-      <c r="Q58" s="12">
+      <c r="Q58" s="7">
         <v>528000</v>
       </c>
     </row>
@@ -7008,8 +6966,1039 @@
         <v>528000</v>
       </c>
     </row>
+    <row r="65" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="12"/>
+      <c r="I66" t="s">
+        <v>20</v>
+      </c>
+      <c r="J66" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="9"/>
+      <c r="C67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="13">
+        <v>3</v>
+      </c>
+      <c r="C68" s="3">
+        <v>1816</v>
+      </c>
+      <c r="D68" s="4">
+        <v>1236</v>
+      </c>
+      <c r="E68" s="4">
+        <v>3930</v>
+      </c>
+      <c r="F68" s="4">
+        <v>5511</v>
+      </c>
+      <c r="G68" s="4">
+        <v>1907</v>
+      </c>
+      <c r="H68" s="4">
+        <v>14400</v>
+      </c>
+      <c r="I68">
+        <f>C68/H68</f>
+        <v>0.12611111111111112</v>
+      </c>
+      <c r="J68">
+        <f>D68/H68</f>
+        <v>8.5833333333333331E-2</v>
+      </c>
+      <c r="K68">
+        <f>I68+J68</f>
+        <v>0.21194444444444444</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="13">
+        <v>5</v>
+      </c>
+      <c r="C69" s="3">
+        <v>1863</v>
+      </c>
+      <c r="D69" s="4">
+        <v>1984</v>
+      </c>
+      <c r="E69" s="4">
+        <v>5554</v>
+      </c>
+      <c r="F69" s="4">
+        <v>10116</v>
+      </c>
+      <c r="G69" s="4">
+        <v>4483</v>
+      </c>
+      <c r="H69" s="4">
+        <v>24000</v>
+      </c>
+      <c r="I69">
+        <f>C69/H69</f>
+        <v>7.7625E-2</v>
+      </c>
+      <c r="J69">
+        <f>D69/H69</f>
+        <v>8.2666666666666666E-2</v>
+      </c>
+      <c r="K69">
+        <f t="shared" ref="K69:K72" si="0">I69+J69</f>
+        <v>0.16029166666666667</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="13">
+        <v>7</v>
+      </c>
+      <c r="C70" s="3">
+        <v>1867</v>
+      </c>
+      <c r="D70" s="4">
+        <v>2234</v>
+      </c>
+      <c r="E70" s="4">
+        <v>7033</v>
+      </c>
+      <c r="F70" s="4">
+        <v>14856</v>
+      </c>
+      <c r="G70" s="4">
+        <v>7610</v>
+      </c>
+      <c r="H70" s="4">
+        <v>33600</v>
+      </c>
+      <c r="I70">
+        <f>C70/H70</f>
+        <v>5.5565476190476193E-2</v>
+      </c>
+      <c r="J70">
+        <f>D70/H70</f>
+        <v>6.6488095238095235E-2</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="0"/>
+        <v>0.12205357142857143</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="13">
+        <v>11</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1867</v>
+      </c>
+      <c r="D71" s="4">
+        <v>2252</v>
+      </c>
+      <c r="E71" s="4">
+        <v>8620</v>
+      </c>
+      <c r="F71" s="4">
+        <v>25452</v>
+      </c>
+      <c r="G71" s="4">
+        <v>14609</v>
+      </c>
+      <c r="H71" s="4">
+        <v>52800</v>
+      </c>
+      <c r="I71">
+        <f>C71/H71</f>
+        <v>3.5359848484848487E-2</v>
+      </c>
+      <c r="J71">
+        <f>D71/H71</f>
+        <v>4.2651515151515149E-2</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="0"/>
+        <v>7.8011363636363629E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="13">
+        <v>110</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1867</v>
+      </c>
+      <c r="D72" s="4">
+        <v>2252</v>
+      </c>
+      <c r="E72" s="4">
+        <v>9086</v>
+      </c>
+      <c r="F72" s="4">
+        <v>89176</v>
+      </c>
+      <c r="G72" s="4">
+        <v>425619</v>
+      </c>
+      <c r="H72" s="4">
+        <v>528000</v>
+      </c>
+      <c r="I72">
+        <f>C72/H72</f>
+        <v>3.5359848484848486E-3</v>
+      </c>
+      <c r="J72">
+        <f>D72/H72</f>
+        <v>4.2651515151515152E-3</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="0"/>
+        <v>7.8011363636363643E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="12"/>
+      <c r="I74" t="s">
+        <v>20</v>
+      </c>
+      <c r="J74" t="s">
+        <v>21</v>
+      </c>
+      <c r="K74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="9"/>
+      <c r="C75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="13">
+        <v>3</v>
+      </c>
+      <c r="C76" s="3">
+        <v>380</v>
+      </c>
+      <c r="D76" s="4">
+        <v>609</v>
+      </c>
+      <c r="E76" s="4">
+        <v>7867</v>
+      </c>
+      <c r="F76" s="4">
+        <v>5544</v>
+      </c>
+      <c r="G76" s="4">
+        <v>0</v>
+      </c>
+      <c r="H76" s="4">
+        <v>14400</v>
+      </c>
+      <c r="I76">
+        <f>C76/H76</f>
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="J76">
+        <f>D76/H76</f>
+        <v>4.2291666666666665E-2</v>
+      </c>
+      <c r="K76">
+        <f>I76+J76</f>
+        <v>6.868055555555555E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="13">
+        <v>5</v>
+      </c>
+      <c r="C77" s="3">
+        <v>380</v>
+      </c>
+      <c r="D77" s="4">
+        <v>609</v>
+      </c>
+      <c r="E77" s="4">
+        <v>12235</v>
+      </c>
+      <c r="F77" s="4">
+        <v>10776</v>
+      </c>
+      <c r="G77" s="4">
+        <v>0</v>
+      </c>
+      <c r="H77" s="4">
+        <v>24000</v>
+      </c>
+      <c r="I77">
+        <f>C77/H77</f>
+        <v>1.5833333333333335E-2</v>
+      </c>
+      <c r="J77">
+        <f>D77/H77</f>
+        <v>2.5375000000000002E-2</v>
+      </c>
+      <c r="K77">
+        <f t="shared" ref="K77:K80" si="1">I77+J77</f>
+        <v>4.1208333333333333E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="13">
+        <v>7</v>
+      </c>
+      <c r="C78" s="3">
+        <v>380</v>
+      </c>
+      <c r="D78" s="4">
+        <v>609</v>
+      </c>
+      <c r="E78" s="4">
+        <v>15472</v>
+      </c>
+      <c r="F78" s="4">
+        <v>17139</v>
+      </c>
+      <c r="G78" s="4">
+        <v>0</v>
+      </c>
+      <c r="H78" s="4">
+        <v>33600</v>
+      </c>
+      <c r="I78">
+        <f>C78/H78</f>
+        <v>1.1309523809523809E-2</v>
+      </c>
+      <c r="J78">
+        <f>D78/H78</f>
+        <v>1.8124999999999999E-2</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="1"/>
+        <v>2.9434523809523806E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="13">
+        <v>11</v>
+      </c>
+      <c r="C79" s="3">
+        <v>380</v>
+      </c>
+      <c r="D79" s="4">
+        <v>609</v>
+      </c>
+      <c r="E79" s="4">
+        <v>20105</v>
+      </c>
+      <c r="F79" s="4">
+        <v>31706</v>
+      </c>
+      <c r="G79" s="4">
+        <v>0</v>
+      </c>
+      <c r="H79" s="4">
+        <v>52800</v>
+      </c>
+      <c r="I79">
+        <f>C79/H79</f>
+        <v>7.1969696969696973E-3</v>
+      </c>
+      <c r="J79">
+        <f>D79/H79</f>
+        <v>1.1534090909090909E-2</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="1"/>
+        <v>1.8731060606060605E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="14">
+        <v>110</v>
+      </c>
+      <c r="C80" s="6">
+        <v>380</v>
+      </c>
+      <c r="D80" s="7">
+        <v>609</v>
+      </c>
+      <c r="E80" s="7">
+        <v>30917</v>
+      </c>
+      <c r="F80" s="7">
+        <v>446624</v>
+      </c>
+      <c r="G80" s="7">
+        <v>49470</v>
+      </c>
+      <c r="H80" s="4">
+        <v>528000</v>
+      </c>
+      <c r="I80">
+        <f>C80/H80</f>
+        <v>7.1969696969696967E-4</v>
+      </c>
+      <c r="J80">
+        <f>D80/H80</f>
+        <v>1.153409090909091E-3</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="1"/>
+        <v>1.8731060606060608E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="12"/>
+      <c r="I82" t="s">
+        <v>20</v>
+      </c>
+      <c r="J82" t="s">
+        <v>21</v>
+      </c>
+      <c r="K82" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="9"/>
+      <c r="C83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="13">
+        <v>3</v>
+      </c>
+      <c r="C84" s="3">
+        <v>792</v>
+      </c>
+      <c r="D84" s="4">
+        <v>900</v>
+      </c>
+      <c r="E84" s="4">
+        <v>2000</v>
+      </c>
+      <c r="F84" s="4">
+        <v>8685</v>
+      </c>
+      <c r="G84" s="4">
+        <v>2023</v>
+      </c>
+      <c r="H84" s="4">
+        <v>14400</v>
+      </c>
+      <c r="I84">
+        <f>C84/H84</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="J84">
+        <f>D84/H84</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K84">
+        <f>I84+J84</f>
+        <v>0.11749999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="13">
+        <v>5</v>
+      </c>
+      <c r="C85" s="3">
+        <v>792</v>
+      </c>
+      <c r="D85" s="4">
+        <v>947</v>
+      </c>
+      <c r="E85" s="4">
+        <v>3111</v>
+      </c>
+      <c r="F85" s="4">
+        <v>14346</v>
+      </c>
+      <c r="G85" s="4">
+        <v>4804</v>
+      </c>
+      <c r="H85" s="4">
+        <v>24000</v>
+      </c>
+      <c r="I85">
+        <f>C85/H85</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="J85">
+        <f>D85/H85</f>
+        <v>3.9458333333333331E-2</v>
+      </c>
+      <c r="K85">
+        <f t="shared" ref="K85:K88" si="2">I85+J85</f>
+        <v>7.2458333333333333E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="13">
+        <v>7</v>
+      </c>
+      <c r="C86" s="3">
+        <v>792</v>
+      </c>
+      <c r="D86" s="4">
+        <v>951</v>
+      </c>
+      <c r="E86" s="4">
+        <v>3704</v>
+      </c>
+      <c r="F86" s="4">
+        <v>19874</v>
+      </c>
+      <c r="G86" s="4">
+        <v>8279</v>
+      </c>
+      <c r="H86" s="4">
+        <v>33600</v>
+      </c>
+      <c r="I86">
+        <f>C86/H86</f>
+        <v>2.3571428571428573E-2</v>
+      </c>
+      <c r="J86">
+        <f>D86/H86</f>
+        <v>2.8303571428571428E-2</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="2"/>
+        <v>5.1875000000000004E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="13">
+        <v>11</v>
+      </c>
+      <c r="C87" s="3">
+        <v>792</v>
+      </c>
+      <c r="D87" s="4">
+        <v>951</v>
+      </c>
+      <c r="E87" s="4">
+        <v>3814</v>
+      </c>
+      <c r="F87" s="4">
+        <v>31005</v>
+      </c>
+      <c r="G87" s="4">
+        <v>16238</v>
+      </c>
+      <c r="H87" s="4">
+        <v>52800</v>
+      </c>
+      <c r="I87">
+        <f>C87/H87</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J87">
+        <f>D87/H87</f>
+        <v>1.8011363636363638E-2</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="2"/>
+        <v>3.3011363636363637E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="13">
+        <v>110</v>
+      </c>
+      <c r="C88" s="3">
+        <v>792</v>
+      </c>
+      <c r="D88" s="4">
+        <v>951</v>
+      </c>
+      <c r="E88" s="4">
+        <v>3814</v>
+      </c>
+      <c r="F88" s="4">
+        <v>74353</v>
+      </c>
+      <c r="G88" s="4">
+        <v>448090</v>
+      </c>
+      <c r="H88" s="4">
+        <v>528000</v>
+      </c>
+      <c r="I88">
+        <f>C88/H88</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="J88">
+        <f>D88/H88</f>
+        <v>1.8011363636363637E-3</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="2"/>
+        <v>3.3011363636363637E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="12"/>
+      <c r="I91" t="s">
+        <v>20</v>
+      </c>
+      <c r="J91" t="s">
+        <v>21</v>
+      </c>
+      <c r="K91" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="9"/>
+      <c r="C92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="3">
+        <v>9280</v>
+      </c>
+      <c r="D93" s="4">
+        <v>9958</v>
+      </c>
+      <c r="E93" s="4">
+        <v>34223</v>
+      </c>
+      <c r="F93" s="4">
+        <v>145111</v>
+      </c>
+      <c r="G93" s="4">
+        <v>454228</v>
+      </c>
+      <c r="H93" s="4">
+        <v>652800</v>
+      </c>
+      <c r="I93">
+        <f>C93/H93</f>
+        <v>1.4215686274509804E-2</v>
+      </c>
+      <c r="J93">
+        <f>D93/H93</f>
+        <v>1.5254289215686275E-2</v>
+      </c>
+      <c r="K93">
+        <f>I93+J93</f>
+        <v>2.9469975490196081E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1900</v>
+      </c>
+      <c r="D94" s="4">
+        <v>3045</v>
+      </c>
+      <c r="E94" s="4">
+        <v>86596</v>
+      </c>
+      <c r="F94" s="4">
+        <v>511789</v>
+      </c>
+      <c r="G94" s="4">
+        <v>49470</v>
+      </c>
+      <c r="H94" s="4">
+        <v>652800</v>
+      </c>
+      <c r="I94">
+        <f>C94/H94</f>
+        <v>2.9105392156862746E-3</v>
+      </c>
+      <c r="J94">
+        <f>D94/H94</f>
+        <v>4.6645220588235293E-3</v>
+      </c>
+      <c r="K94">
+        <f t="shared" ref="K94:K95" si="3">I94+J94</f>
+        <v>7.5750612745098039E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="3">
+        <v>3960</v>
+      </c>
+      <c r="D95" s="4">
+        <v>4700</v>
+      </c>
+      <c r="E95" s="4">
+        <v>16443</v>
+      </c>
+      <c r="F95" s="4">
+        <v>148263</v>
+      </c>
+      <c r="G95" s="4">
+        <v>479434</v>
+      </c>
+      <c r="H95" s="4">
+        <v>652800</v>
+      </c>
+      <c r="I95">
+        <f>C95/H95</f>
+        <v>6.0661764705882354E-3</v>
+      </c>
+      <c r="J95">
+        <f>D95/H95</f>
+        <v>7.1997549019607839E-3</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="3"/>
+        <v>1.3265931372549019E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="12"/>
+      <c r="I97" t="s">
+        <v>20</v>
+      </c>
+      <c r="J97" t="s">
+        <v>21</v>
+      </c>
+      <c r="K97" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="9"/>
+      <c r="C98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="13">
+        <v>3</v>
+      </c>
+      <c r="C99" s="3">
+        <v>2988</v>
+      </c>
+      <c r="D99" s="4">
+        <v>2745</v>
+      </c>
+      <c r="E99" s="4">
+        <v>13797</v>
+      </c>
+      <c r="F99" s="4">
+        <v>19740</v>
+      </c>
+      <c r="G99" s="4">
+        <v>3930</v>
+      </c>
+      <c r="H99" s="4">
+        <v>43200</v>
+      </c>
+      <c r="I99">
+        <f>C99/H99</f>
+        <v>6.9166666666666668E-2</v>
+      </c>
+      <c r="J99">
+        <f>D99/H99</f>
+        <v>6.3541666666666663E-2</v>
+      </c>
+      <c r="K99">
+        <f>I99+J99</f>
+        <v>0.13270833333333332</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="13">
+        <v>5</v>
+      </c>
+      <c r="C100" s="3">
+        <v>3035</v>
+      </c>
+      <c r="D100" s="4">
+        <v>3540</v>
+      </c>
+      <c r="E100" s="4">
+        <v>20900</v>
+      </c>
+      <c r="F100" s="4">
+        <v>35238</v>
+      </c>
+      <c r="G100" s="4">
+        <v>9287</v>
+      </c>
+      <c r="H100" s="4">
+        <v>72000</v>
+      </c>
+      <c r="I100">
+        <f>C100/H100</f>
+        <v>4.2152777777777775E-2</v>
+      </c>
+      <c r="J100">
+        <f>D100/H100</f>
+        <v>4.9166666666666664E-2</v>
+      </c>
+      <c r="K100">
+        <f t="shared" ref="K100:K103" si="4">I100+J100</f>
+        <v>9.1319444444444439E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="13">
+        <v>7</v>
+      </c>
+      <c r="C101" s="3">
+        <v>3039</v>
+      </c>
+      <c r="D101" s="4">
+        <v>3794</v>
+      </c>
+      <c r="E101" s="4">
+        <v>26209</v>
+      </c>
+      <c r="F101" s="4">
+        <v>51869</v>
+      </c>
+      <c r="G101" s="4">
+        <v>15889</v>
+      </c>
+      <c r="H101" s="4">
+        <v>100800</v>
+      </c>
+      <c r="I101">
+        <f>C101/H101</f>
+        <v>3.0148809523809522E-2</v>
+      </c>
+      <c r="J101">
+        <f>D101/H101</f>
+        <v>3.7638888888888888E-2</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="4"/>
+        <v>6.7787698412698411E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="13">
+        <v>11</v>
+      </c>
+      <c r="C102" s="3">
+        <v>3039</v>
+      </c>
+      <c r="D102" s="4">
+        <v>3812</v>
+      </c>
+      <c r="E102" s="4">
+        <v>32539</v>
+      </c>
+      <c r="F102" s="4">
+        <v>88163</v>
+      </c>
+      <c r="G102" s="4">
+        <v>30847</v>
+      </c>
+      <c r="H102" s="4">
+        <v>158400</v>
+      </c>
+      <c r="I102">
+        <f>C102/H102</f>
+        <v>1.9185606060606059E-2</v>
+      </c>
+      <c r="J102">
+        <f>D102/H102</f>
+        <v>2.4065656565656564E-2</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="4"/>
+        <v>4.3251262626262624E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="13">
+        <v>110</v>
+      </c>
+      <c r="C103" s="3">
+        <v>3039</v>
+      </c>
+      <c r="D103" s="4">
+        <v>3812</v>
+      </c>
+      <c r="E103" s="4">
+        <v>43817</v>
+      </c>
+      <c r="F103" s="4">
+        <v>610153</v>
+      </c>
+      <c r="G103" s="4">
+        <v>923179</v>
+      </c>
+      <c r="H103" s="4">
+        <v>1584000</v>
+      </c>
+      <c r="I103">
+        <f>C103/H103</f>
+        <v>1.9185606060606061E-3</v>
+      </c>
+      <c r="J103">
+        <f>D103/H103</f>
+        <v>2.4065656565656567E-3</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="4"/>
+        <v>4.3251262626262631E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="32">
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:H97"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:G82"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:Q50"/>
@@ -7025,7 +8014,6 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:W2"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:H32"/>
@@ -7033,7 +8021,7 @@
     <mergeCell ref="K32:K33"/>
     <mergeCell ref="L32:Q32"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="B66:B67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>